<commit_message>
Update S3 prefix and add Neo4j loading
</commit_message>
<xml_diff>
--- a/sdtm_workspace/mapping_specs/ae_mapping_specification.xlsx
+++ b/sdtm_workspace/mapping_specs/ae_mapping_specification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,7 +519,7 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Required variable. Study identifier from STUDY column (MAXIS-08)</t>
+          <t>Study Identifier - Required variable. Maps from STUDY source column containing 'MAXIS-08'</t>
         </is>
       </c>
     </row>
@@ -558,7 +558,7 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Required variable. Domain abbreviation for Adverse Events</t>
+          <t>Domain Abbreviation - Required variable. Fixed value for Adverse Events domain</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Required variable. Unique subject identifier. Need to extract subject ID from source data structure</t>
+          <t>Unique Subject Identifier - Required variable. Standard derivation combining study, site, and subject identifiers. INVSITE present in source.</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Use source value if valid, otherwise derive</t>
+          <t>Use as-is if valid, otherwise regenerate</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -640,7 +640,7 @@
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Required variable. Sequence number per subject. Source has AESEQ column but should validate sequential ordering</t>
+          <t>Sequence Number - Required variable. Source has AESEQ column. Validate and regenerate if needed to ensure sequential ordering per subject</t>
         </is>
       </c>
     </row>
@@ -667,12 +667,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>AEVERB</t>
+          <t>AECOD</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>COPY(AEVERB)</t>
+          <t>Use reported term as-is</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -683,7 +683,7 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Required variable. Reported term for adverse event as recorded by investigator</t>
+          <t>Reported Term for the Adverse Event - Required variable. AECOD contains verbatim terms like 'NAUSEA', 'INTERMITTENT VOMITING', etc.</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>COPY(AEPTT)</t>
+          <t>Use MedDRA Preferred Term</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -725,12 +725,12 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>MedDRA Preferred Term</t>
+          <t>MedDRA</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Expected variable. Dictionary-derived term (MedDRA Preferred Term)</t>
+          <t>Dictionary-Derived Term - Expected variable. AEPTT contains MedDRA Preferred Terms like 'NAUSEA', 'VOMITING', 'BACK PAIN'</t>
         </is>
       </c>
     </row>
@@ -762,7 +762,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>COPY(AESCT)</t>
+          <t>Use MedDRA System Organ Class</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -772,12 +772,12 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>MedDRA SOC</t>
+          <t>MedDRA</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Expected variable. Body System or Organ Class from MedDRA SOC</t>
+          <t>Body System or Organ Class - Expected variable. AESCT contains SOC terms like 'GASTROINTESTINAL DISORDERS'</t>
         </is>
       </c>
     </row>
@@ -809,101 +809,101 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Same as AEBODSYS</t>
+          <t>Use MedDRA Primary System Organ Class</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>DERIVE</t>
+          <t>COPY</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>MedDRA SOC</t>
+          <t>MedDRA</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Permissible variable. Primary System Organ Class</t>
+          <t>Primary System Organ Class - Permissible variable. Same as AEBODSYS for primary SOC</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>AESOCCD</t>
+          <t>AESEV</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Primary System Organ Class Code</t>
+          <t>Severity/Intensity</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Num</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Perm</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>AESCC</t>
+          <t>AESEV</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Convert to numeric</t>
+          <t>Map to CDISC controlled terminology: Keep MILD/MODERATE/SEVERE as-is</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>COPY</t>
+          <t>MAP</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>MedDRA SOC Code</t>
+          <t>AESEV</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Permissible variable. Primary System Organ Class Code</t>
+          <t>Severity/Intensity - Expected variable. Source already contains CDISC terms (MILD, MODERATE, SEVERE). Validate against AESEV codelist</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>AEPTCD</t>
+          <t>AESER</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Preferred Term Code</t>
+          <t>Serious Event</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Num</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Perm</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>AEPTC</t>
+          <t>AESER</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Convert to numeric</t>
+          <t>Validate against NY codelist</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -913,24 +913,24 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>MedDRA PT Code</t>
+          <t>NY</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Permissible variable. Preferred Term Code from MedDRA</t>
+          <t>Serious Event - Expected variable. Source has AESER column. Ensure values are Y or N only</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>AEHLT</t>
+          <t>AEACN</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>High Level Term</t>
+          <t>Action Taken with Study Treatment</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -940,91 +940,91 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Perm</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>AEHTT</t>
+          <t>AEACT</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>COPY(AEHTT)</t>
+          <t>Map to ACN codelist</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>COPY</t>
+          <t>MAP</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>MedDRA HLT</t>
+          <t>ACN</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Permissible variable. High Level Term from MedDRA</t>
+          <t>Action Taken with Study Treatment - Expected variable. AEACT contains action taken information. Map to standard ACN values (DOSE REDUCED, DOSE NOT CHANGED, DRUG WITHDRAWN, etc.)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AEHLTCD</t>
+          <t>AEREL</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>High Level Term Code</t>
+          <t>Causality</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Num</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Perm</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>AEHTC</t>
+          <t>AEREL</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Convert to numeric</t>
+          <t>Map to AEREL codelist</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>COPY</t>
+          <t>MAP</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>MedDRA HLT Code</t>
+          <t>AEREL</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Permissible variable. High Level Term Code</t>
+          <t>Causality - Expected variable. Source has both AEREL and AERELL. Map values like 'POSSIBLE', 'UNLIKELY', 'UNRELATED' to AEREL codelist (NOT RELATED, POSSIBLY RELATED, PROBABLY RELATED, RELATED)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AEHLGT</t>
+          <t>AEOUT</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>High Level Group Term</t>
+          <t>Outcome of Adverse Event</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1034,91 +1034,87 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Perm</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>AEHGT1</t>
+          <t>AEOUTC</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>COPY(AEHGT1)</t>
+          <t>Map to OUT codelist</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>COPY</t>
+          <t>MAP</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>MedDRA HLGT</t>
+          <t>OUT</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Permissible variable. High Level Group Term (source column appears empty)</t>
+          <t>Outcome of Adverse Event - Expected variable. Source has AEOUTC and AEOUTCL. AEOUTCL shows 'RESOLVED'. Map to OUT codelist (RECOVERED/RESOLVED, RECOVERING/RESOLVING, NOT RECOVERED/NOT RESOLVED, FATAL, UNKNOWN)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>AEHLGTCD</t>
+          <t>AESTDTC</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>High Level Group Term Code</t>
+          <t>Start Date/Time of Adverse Event</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Num</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Perm</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>AEHGC</t>
+          <t>AESTDT</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Convert to numeric</t>
+          <t>Convert to ISO 8601 format</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>COPY</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>MedDRA HLGT Code</t>
-        </is>
-      </c>
+          <t>DATE_FORMAT</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Permissible variable. High Level Group Term Code</t>
+          <t>Start Date/Time of Adverse Event - Expected variable. Source has numeric dates (20080910, 200812). Convert to ISO 8601 format preserving precision</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>AELLT</t>
+          <t>AEENDTC</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Lowest Level Term</t>
+          <t>End Date/Time of Adverse Event</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1128,49 +1124,45 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Perm</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>AELTT</t>
+          <t>AEENDT</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>COPY(AELTT)</t>
+          <t>Convert to ISO 8601 format</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>COPY</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>MedDRA LLT</t>
-        </is>
-      </c>
+          <t>DATE_FORMAT</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Permissible variable. Lowest Level Term from MedDRA</t>
+          <t>End Date/Time of Adverse Event - Expected variable. Source has numeric dates with some nulls. Convert to ISO 8601 format preserving precision</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>AELLTCD</t>
+          <t>AESPID</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Lowest Level Term Code</t>
+          <t>Sponsor-Defined Identifier</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Num</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1180,39 +1172,35 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>AELTC</t>
+          <t>PrimaryKEY</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Convert to numeric</t>
+          <t>Convert to character</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>COPY</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>MedDRA LLT Code</t>
-        </is>
-      </c>
+          <t>DERIVE</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Permissible variable. Lowest Level Term Code</t>
+          <t>Sponsor-Defined Identifier - Permissible variable. PrimaryKEY can serve as unique AE identifier within the study</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>AESEV</t>
+          <t>AEMODIFY</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Severity/Intensity</t>
+          <t>Modified Reported Term</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1222,96 +1210,92 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>AESEV</t>
+          <t>AEVERB</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Map to CDISC controlled terminology: MILD-&gt;MILD, MODERATE-&gt;MODERATE, SEVERE-&gt;SEVERE</t>
+          <t>Use if different from AETERM</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>MAP</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>AESEV</t>
-        </is>
-      </c>
+          <t>DERIVE</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Expected variable. Severity/Intensity. Source already contains MILD/MODERATE/SEVERE values</t>
+          <t>Modified Reported Term - Permissible variable. AEVERB may contain investigator-modified verbatim term</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>AESER</t>
+          <t>AESOCCD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Serious Event</t>
+          <t>Primary System Organ Class Code</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t>Num</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>AESER</t>
+          <t>AESCC</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Map Y-&gt;Y, N-&gt;N</t>
+          <t>Convert to numeric</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>MAP</t>
+          <t>DERIVE</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>MedDRA</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Expected variable. Serious Event flag (Yes/No)</t>
+          <t>Primary System Organ Class Code - Permissible variable. MedDRA SOC numeric code</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AESLIFE</t>
+          <t>AEHLGTCD</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Is Life Threatening</t>
+          <t>High Level Group Term Code</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t>Num</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1321,39 +1305,39 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>AESERL</t>
+          <t>AEHGC</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Map to Y/N codelist</t>
+          <t>Convert to numeric</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>MAP</t>
+          <t>DERIVE</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>MedDRA</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Expected variable. Is event life threatening</t>
+          <t>High Level Group Term Code - Permissible variable. MedDRA HLGT numeric code</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>AEACN</t>
+          <t>AEHLGT</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Action Taken with Study Treatment</t>
+          <t>High Level Group Term</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1363,49 +1347,49 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>AEACT</t>
+          <t>AEHGT1</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Map to ACN codelist values</t>
+          <t>Use MedDRA HLGT term</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>MAP</t>
+          <t>COPY</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>ACN</t>
+          <t>MedDRA</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Expected variable. Action taken with study treatment</t>
+          <t>High Level Group Term - Permissible variable. All values are null in sample, may be populated in full dataset</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>AEACNOTH</t>
+          <t>AEHLTCD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Other Action Taken</t>
+          <t>High Level Term Code</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t>Num</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1415,35 +1399,39 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>AEACTL</t>
+          <t>AEHTC</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>COPY(AEACTL)</t>
+          <t>Convert to numeric</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>COPY</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr"/>
+          <t>DERIVE</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>MedDRA</t>
+        </is>
+      </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Permissible variable. Other action taken (free text description)</t>
+          <t>High Level Term Code - Permissible variable. MedDRA HLT numeric code</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AEREL</t>
+          <t>AEHLT</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Causality</t>
+          <t>High Level Term</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1453,91 +1441,91 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>AEREL</t>
+          <t>AEHTT</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Map source values to AEREL codelist: POSSIBLE-&gt;POSSIBLE, UNLIKELY-&gt;UNLIKELY, UNRELATED-&gt;NOT RELATED</t>
+          <t>Use MedDRA HLT term</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>MAP</t>
+          <t>COPY</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>AEREL</t>
+          <t>MedDRA</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Expected variable. Causality/relationship to study treatment</t>
+          <t>High Level Term - Permissible variable. AEHTT contains terms like 'NAUSEA AND VOMITING SYMPTOMS'</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>AEREL</t>
+          <t>AELLTCD</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Causality</t>
+          <t>Lowest Level Term Code</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t>Num</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>AERELL</t>
+          <t>AELTC</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Map: POSSIBLE-&gt;POSSIBLE, UNLIKELY-&gt;UNLIKELY, UNRELATED-&gt;NOT RELATED, PROBABLE-&gt;PROBABLE, RELATED-&gt;RELATED</t>
+          <t>Convert to numeric</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>MAP</t>
+          <t>DERIVE</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>AEREL</t>
+          <t>MedDRA</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Alternative causality field (AERELL appears to be the populated field based on sample data)</t>
+          <t>Lowest Level Term Code - Permissible variable. MedDRA LLT numeric code</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>AEOUT</t>
+          <t>AELLT</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Outcome of Adverse Event</t>
+          <t>Lowest Level Term</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1547,91 +1535,91 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>AEOUTC</t>
+          <t>AELTT</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Map to OUT codelist values</t>
+          <t>Use MedDRA LLT term</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>MAP</t>
+          <t>COPY</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>OUT</t>
+          <t>MedDRA</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Expected variable. Outcome of adverse event</t>
+          <t>Lowest Level Term - Permissible variable. MedDRA Lowest Level Term</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>AEOUT</t>
+          <t>AEPTCD</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Outcome of Adverse Event</t>
+          <t>Preferred Term Code</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t>Num</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>AEOUTCL</t>
+          <t>AEPTC</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Map RESOLVED-&gt;RECOVERED/RESOLVED, map to standard OUT codelist</t>
+          <t>Convert to numeric</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>MAP</t>
+          <t>DERIVE</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>OUT</t>
+          <t>MedDRA</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Alternative outcome field. AEOUTCL appears populated with values like RESOLVED</t>
+          <t>Preferred Term Code - Permissible variable. MedDRA PT numeric code corresponding to AEPTT</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>AESTDTC</t>
+          <t>AEACNOTH</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Start Date/Time of Adverse Event</t>
+          <t>Other Action Taken</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1641,45 +1629,45 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>AESTDT</t>
+          <t>AEACTL</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Convert numeric date format to ISO 8601: YYYYMMDD-&gt;YYYY-MM-DD, YYYYMM-&gt;YYYY-MM, YYYY-&gt;YYYY</t>
+          <t>Use for other actions taken</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>COPY</t>
+          <t>DERIVE</t>
         </is>
       </c>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Expected variable. Start date of adverse event in ISO 8601 format. Handle partial dates appropriately</t>
+          <t>Other Action Taken - Permissible variable. Free text for actions not covered by AEACN codelist</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>AESTDY</t>
+          <t>AEPATT</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Study Day of Start of Adverse Event</t>
+          <t>Pattern of Adverse Event</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Num</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1689,35 +1677,35 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>AESTDT</t>
+          <t>AEPTT</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Calculate study day: AESTDT - Treatment Start Date + 1 (if AESTDT &gt;= TRT Start), else AESTDT - Treatment Start Date</t>
+          <t>Derive pattern if applicable</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>DATE_FORMAT</t>
+          <t>DERIVE</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Permissible variable. Study day of start of adverse event relative to treatment start</t>
+          <t>Pattern of Adverse Event - Permissible variable. May need derivation logic based on recurrence and temporal patterns</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>AEENDTC</t>
+          <t>AESDTH</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>End Date/Time of Adverse Event</t>
+          <t>Results in Death</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1727,45 +1715,45 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>AEENDT</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Convert numeric date format to ISO 8601: YYYYMMDD-&gt;YYYY-MM-DD, YYYYMM-&gt;YYYY-MM, YYYY-&gt;YYYY</t>
-        </is>
-      </c>
+          <t>[derived]</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>COPY</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr"/>
+          <t>DERIVE</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>NY</t>
+        </is>
+      </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Expected variable. End date of adverse event in ISO 8601 format. Handle partial dates and nulls</t>
+          <t>Results in Death - Expected variable. Derive from seriousness criteria. Check AESERL for death indicator</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>AEENDY</t>
+          <t>AESHOSP</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Study Day of End of Adverse Event</t>
+          <t>Requires or Prolongs Hospitalization</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Num</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1775,35 +1763,35 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>AEENDT</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>Calculate study day: AEENDT - Treatment Start Date + 1 (if AEENDT &gt;= TRT Start), else AEENDT - Treatment Start Date</t>
-        </is>
-      </c>
+          <t>[derived]</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>DATE_FORMAT</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr"/>
+          <t>DERIVE</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>NY</t>
+        </is>
+      </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Permissible variable. Study day of end of adverse event relative to treatment start</t>
+          <t>Requires or Prolongs Hospitalization - Expected variable. Check AESERL for hospitalization indicator</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>AEDTC</t>
+          <t>AESLIFE</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Date/Time of Collection</t>
+          <t>Is Life Threatening</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1818,40 +1806,40 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>AESTDT</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Use AESTDTC value</t>
-        </is>
-      </c>
+          <t>[derived]</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
           <t>DERIVE</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr"/>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>NY</t>
+        </is>
+      </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Permissible variable. Date/Time of adverse event collection (typically same as start date)</t>
+          <t>Is Life Threatening - Expected variable. Check AESERL for life-threatening indicator</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>AEDY</t>
+          <t>AESDISAB</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>AEDY</t>
+          <t>Persist or Signif Disability/Incapacity</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Num</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1861,35 +1849,35 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>AESTDT</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Set equal to AESTDY</t>
-        </is>
-      </c>
+          <t>[derived]</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
           <t>DERIVE</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr"/>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>NY</t>
+        </is>
+      </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Permissible variable. Study day of adverse event collection</t>
+          <t>Persist or Signif Disability/Incapacity - Expected variable. Check AESERL for disability indicator</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>AECONTRT</t>
+          <t>AESCONG</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Concomitant or Additional Trtmnt Given</t>
+          <t>Congenital Anomaly or Birth Defect</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1904,17 +1892,13 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>AETRT</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Map Y-&gt;Y, N-&gt;N</t>
-        </is>
-      </c>
+          <t>[derived]</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>MAP</t>
+          <t>DERIVE</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1924,19 +1908,19 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Permissible variable. Concomitant or Additional Treatment Given</t>
+          <t>Congenital Anomaly or Birth Defect - Expected variable. Check AESERL for congenital anomaly indicator</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>AESITE</t>
+          <t>AESMIE</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>AESITE</t>
+          <t>Other Medically Important Serious Event</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1951,35 +1935,35 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>INVSITE</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>COPY(INVSITE)</t>
-        </is>
-      </c>
+          <t>[derived]</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>COPY</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr"/>
+          <t>DERIVE</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>NY</t>
+        </is>
+      </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Permissible variable. Investigational site identifier (if AESITE is used for site location)</t>
+          <t>Other Medically Important Serious Event - Expected variable. Check AESERL for other medically important criteria</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>AESPID</t>
+          <t>AECONTRT</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Sponsor-Defined Identifier</t>
+          <t>Concomitant or Additional Trtmnt Given</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1994,35 +1978,39 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>PrimaryKEY</t>
+          <t>AETRT</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Convert to character</t>
+          <t>Map Y/N to controlled terminology</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>COPY</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr"/>
+          <t>MAP</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>NY</t>
+        </is>
+      </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>Permissible variable. Sponsor-defined identifier (unique event identifier from EDC)</t>
+          <t>Concomitant or Additional Trtmnt Given - Permissible variable. AETRT indicates if treatment was given (Y/N)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>AETERM</t>
+          <t>VISIT</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Reported Term for the Adverse Event</t>
+          <t>Visit Name</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2032,45 +2020,45 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Req</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>DCMNAME</t>
+          <t>VISIT</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Use as supplemental source if AEVERB is empty</t>
+          <t>Use as-is</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>DERIVE</t>
+          <t>COPY</t>
         </is>
       </c>
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Alternative source for reported term if needed</t>
+          <t>Visit Name - SDTM Timing variable. Links AE to visit structure if applicable</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>AESDTH</t>
+          <t>AESTDY</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Results in Death</t>
+          <t>Study Day of Start of Adverse Event</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t>Num</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2086,34 +2074,30 @@
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>DERIVE</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>NY</t>
-        </is>
-      </c>
+          <t>DATE_FORMAT</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Expected variable. Results in death flag (derive from serious event criteria if not in source)</t>
+          <t>Study Day of Start of Adverse Event - Permissible variable. Requires reference start date from DM domain</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>AESHOSP</t>
+          <t>AEENDY</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Requires or Prolongs Hospitalization</t>
+          <t>Study Day of End of Adverse Event</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t>Num</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -2129,29 +2113,25 @@
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>DERIVE</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>NY</t>
-        </is>
-      </c>
+          <t>DATE_FORMAT</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Expected variable. Requires or prolongs hospitalization (derive from serious event criteria if not in source)</t>
+          <t>Study Day of End of Adverse Event - Permissible variable. Requires reference start date from DM domain</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>AESDISAB</t>
+          <t>AERELNST</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Persist or Signif Disability/Incapacity</t>
+          <t>Relationship to Non-Study Treatment</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2166,35 +2146,39 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>[derived]</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr"/>
+          <t>AERELL</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Map to AEREL codelist for non-study treatment relationship</t>
+        </is>
+      </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>DERIVE</t>
+          <t>MAP</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>AEREL</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Expected variable. Persist or significant disability/incapacity (derive from serious event criteria)</t>
+          <t>Causality for Non-Study Treatment - Permissible variable. AERELL may represent relationship to non-study treatment if study tracks this separately</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>AESCONG</t>
+          <t>AEREPNUM</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Congenital Anomaly or Birth Defect</t>
+          <t>AEREPNUM</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2209,35 +2193,35 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[derived]</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr"/>
+          <t>REPEATSN</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Convert to numeric</t>
+        </is>
+      </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>DERIVE</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>NY</t>
-        </is>
-      </c>
+          <t>COPY</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Expected variable. Congenital anomaly or birth defect (derive from serious event criteria)</t>
+          <t>Repeat Number - Permissible variable. REPEATSN may indicate repeat occurrence number for recurring events</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>AESMIE</t>
+          <t>AESUBEV</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Other Medically Important Serious Event</t>
+          <t>AESUBEV</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2252,500 +2236,23 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>[derived]</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr"/>
+          <t>SUBEVE</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Use as-is</t>
+        </is>
+      </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>DERIVE</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>NY</t>
-        </is>
-      </c>
+          <t>COPY</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr">
         <is>
-          <t>Expected variable. Other medically important serious event (derive from serious event criteria)</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>VISIT</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Visit Name</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Perm</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>VISIT</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>COPY(VISIT)</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>COPY</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>SDTM Timing variable. Visit name (can be used for supplemental context, not part of core AE domain)</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>AESEQ</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Sequence Number</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Num</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Req</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>REPEATSN</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Use as alternative or validation for sequence number if AESEQ is not reliable</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>DERIVE</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>May represent repeat or sequence information from EDC</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>AEPRESP</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Pre-Specified Adverse Event</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Perm</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>AEANYL</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>Map to Y/N</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>MAP</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>NY</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>Permissible variable. Pre-specified adverse event of special interest (if AEANYL indicates analysis flag)</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>AEMODIFY</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Modified Reported Term</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Perm</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>QUALIFYV</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>COPY(QUALIFYV)</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>COPY</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>Permissible variable. Modified reported term (if source contains modified or qualified term)</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>SUPPAE.QVAL</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>SUPPAE.QVAL</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Perm</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>AEQS1</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>Create SUPPAE record with QNAM='AEQS1'</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>DERIVE</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>Supplemental qualifier - appears to be study-specific question. Map to SUPPAE domain</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>SUPPAE.QVAL</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>SUPPAE.QVAL</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Perm</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>SUBEVE</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>Create SUPPAE record with QNAM='SUBEVE'</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>DERIVE</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr"/>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>Supplemental qualifier - sub-event information. Map to SUPPAE domain</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>SUPPAE.QVAL</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>SUPPAE.QVAL</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Perm</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>CPEVENT</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>Create SUPPAE record with QNAM='CPEVENT' if needed for traceability</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>DERIVE</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>Supplemental qualifier - case report page event type. Map to SUPPAE if needed</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>SUPPAE.QVAL</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>SUPPAE.QVAL</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Perm</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>Create SUPPAE record with QNAM='PT' if represents additional preferred term version</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>DERIVE</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>May represent preferred term version or alternative coding. Sample shows '1-Jan' which may be version date</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>SUPPAE.QVAL</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>SUPPAE.QVAL</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Perm</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>AECOD</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>Create SUPPAE record with QNAM='AECOD' if represents alternative coding system</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>DERIVE</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>Alternative or legacy coding field - contains terms similar to AEVERB. Map to SUPPAE if needed for traceability</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>AEOCCUR</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Adverse Event Occurrence</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Perm</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>[derived]</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>DERIVE</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>NY</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>Permissible variable. Adverse Event Occurrence flag - always Y in AE domain</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>EPOCH</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Epoch</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Perm</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>[derived]</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>DATE_FORMAT</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>EPOCH</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>SDTM Timing variable. Trial epoch during which AE occurred</t>
+          <t>Sub-Event - Permissible variable. SUBEVE may indicate this is a sub-event of a parent event</t>
         </is>
       </c>
     </row>
@@ -2848,7 +2355,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2026-01-27T17:03:45.223293</t>
+          <t>2026-01-31T23:41:05.684896</t>
         </is>
       </c>
     </row>
@@ -2875,7 +2382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2970,12 +2477,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>AESOC</t>
+          <t>AESEV</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Same as AEBODSYS</t>
+          <t>Apply BR-AE-003: Map 1/MILD -&gt; MILD, 2/MODERATE -&gt; MODERATE, 3/SEVERE -&gt; SEVERE</t>
         </is>
       </c>
     </row>
@@ -2987,7 +2494,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Use AERELL as primary source if AEREL is not populated or for validation</t>
+          <t>Use AEREL if present, otherwise use AERELL as fallback</t>
         </is>
       </c>
     </row>
@@ -2999,139 +2506,223 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Use AEOUTCL as primary source, map to standard terminology</t>
+          <t>Use AEOUTC if present, otherwise use AEOUTCL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>AEDTC</t>
+          <t>AESTDTC</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Set equal to AESTDTC</t>
+          <t>Convert AESTDT from numeric YYYYMMDD or YYYYMM format to ISO 8601 (YYYY-MM-DD or YYYY-MM). Handle partial dates: 200812 -&gt; 2008-12, 20080910 -&gt; 2008-09-10</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>AEDY</t>
+          <t>AEENDTC</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Set equal to AESTDY</t>
+          <t>Convert AEENDT from numeric YYYYMMDD or YYYYMM format to ISO 8601 (YYYY-MM-DD or YYYY-MM). Handle partial dates and nulls (148 null values present)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AETERM</t>
+          <t>AESPID</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Use as supplemental source if AEVERB is empty</t>
+          <t>Convert numeric PrimaryKEY to character string</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AESDTH</t>
+          <t>AEMODIFY</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Derive from AESER and seriousness criteria: if death occurred, set to Y, else N</t>
+          <t>Populate only if AEVERB differs from AECOD, indicating modified term</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>AESHOSP</t>
+          <t>AESOCCD</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Derive from AESER and seriousness criteria: if hospitalization occurred, set to Y, else N</t>
+          <t>Convert AESCC to numeric MedDRA SOC code</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>AESDISAB</t>
+          <t>AEHLGTCD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Derive from AESER and seriousness criteria: if disability occurred, set to Y, else N</t>
+          <t>Convert AEHGC to numeric MedDRA HLGT code</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>AESCONG</t>
+          <t>AEHLTCD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Derive from AESER and seriousness criteria: if congenital anomaly, set to Y, else N</t>
+          <t>Convert AEHTC to numeric MedDRA HLT code</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>AESMIE</t>
+          <t>AELLTCD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Derive from AESER and seriousness criteria: if other medically important event, set to Y, else N</t>
+          <t>Convert AELTC to numeric MedDRA LLT code</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SUPPAE.QVAL</t>
+          <t>AEPTCD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Create SUPPAE record with QNAM='AEQS1'</t>
+          <t>Convert AEPTC to numeric MedDRA PT code</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AEOCCUR</t>
+          <t>AEACNOTH</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Set to 'Y' for all records (since these are adverse events that occurred)</t>
+          <t>Populate when action taken is 'OTHER' with description from AEACTL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>EPOCH</t>
+          <t>AEPATT</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Derive from visit date/treatment dates: map to TREATMENT, FOLLOW-UP, etc. based on timing</t>
+          <t>Analyze multiple records per subject to identify patterns (INTERMITTENT, CONTINUOUS, SINGLE EVENT)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>AESDTH</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Derive from AESER='Y' and AEOUT='FATAL' or AESERL serious criteria</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>AESHOSP</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Derive from AESERL serious criteria for hospitalization</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>AESLIFE</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Derive from AESERL serious criteria for life-threatening</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>AESDISAB</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Derive from AESERL serious criteria for disability</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>AESCONG</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Derive from AESERL serious criteria for congenital anomaly</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>AESMIE</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Derive from AESERL serious criteria for medically important event</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Use AERELL if tracking relationship to non-study treatment separately</t>
         </is>
       </c>
     </row>
@@ -3146,7 +2737,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3893,6 +3484,270 @@
         </is>
       </c>
       <c r="B62" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>,</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>,</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>AERELNST</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
         <is>
           <t>E</t>
         </is>

</xml_diff>